<commit_message>
Cleanup and Final Run
</commit_message>
<xml_diff>
--- a/Plots/top10marker_high.xlsx
+++ b/Plots/top10marker_high.xlsx
@@ -518,251 +518,251 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>vascular smooth muscle cells</t>
+          <t>immune plasma cells</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>9.551122738173099</v>
+        <v>9.085298560672895</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>immune plasma cells</t>
+          <t>brain inhibitory neurons</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>9.085298560672895</v>
+        <v>8.345653939886271</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>brain inhibitory neurons</t>
+          <t>vascular schwann cells</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>8.345653939886271</v>
+        <v>7.797791580400276</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>vascular schwann cells</t>
+          <t>testis late spermatids</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>7.797791580400276</v>
+        <v>7.707802141764406</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>testis late spermatids</t>
+          <t>eye cone photoreceptor cells</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>7.707802141764406</v>
+        <v>6.935374149659864</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>eye cone photoreceptor cells</t>
+          <t>kidney proximal tubular cells</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>6.935374149659864</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>kidney proximal tubular cells</t>
+          <t>brain oligodendrocytes</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>6.5</v>
+        <v>6.22508038585209</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>brain oligodendrocytes</t>
+          <t>liver hepatocytes</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>6.22508038585209</v>
+        <v>5.703277488614184</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>liver hepatocytes</t>
+          <t>small intestine proximal enterocytes</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>5.703277488614184</v>
+        <v>5.586423097762984</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>small intestine proximal enterocytes</t>
+          <t>immune granulocytes</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>5.586423097762984</v>
+        <v>5.460869565217391</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>immune granulocytes</t>
+          <t>eye muller glia cells</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>5.460869565217391</v>
+        <v>5.38448275862069</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>eye muller glia cells</t>
+          <t>brain oligodendrocyte precursor cells</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>5.38448275862069</v>
+        <v>5.045883206383751</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>brain oligodendrocyte precursor cells</t>
+          <t>lung alveolar cells type 2</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>5.045883206383751</v>
+        <v>4.392384105960265</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>skin smooth muscle cells</t>
+          <t>colon distal enterocytes</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>5.032843137254902</v>
+        <v>3.729681404421326</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>esophagus schwann cells</t>
+          <t>tongue basal keratinocytes</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>4.991666666666666</v>
+        <v>3.453606599948063</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>breast fibroblasts</t>
+          <t>immune macrophages</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>4.855421686746987</v>
+        <v>3.26603325415677</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>bronchus ciliated cells</t>
+          <t>brain astrocytes</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>4.692307692307693</v>
+        <v>3.195402298850575</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>lung alveolar cells type 2</t>
+          <t>adipose tissue schwann cells</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>4.392384105960265</v>
+        <v>3.16411842686699</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>colon distal enterocytes</t>
+          <t>fallopian tube neutrophils</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>3.89247311827957</v>
+        <v>3.112192860454335</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>lung alveolar cells type 1</t>
+          <t>placenta syncytiotrophoblasts</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>3.772613182113972</v>
+        <v>2.881351200446677</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>immune dendritic cells</t>
+          <t>colon undifferentiated cells</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>3.682410423452769</v>
+        <v>2.772928526249209</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>tongue basal keratinocytes</t>
+          <t>breast breast glandular cells</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>3.453606599948063</v>
+        <v>2.622448979591837</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>placenta smooth muscle cells</t>
+          <t>esophagus schwann cells</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>3.278140293637847</v>
+        <v>2.608695652173913</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>brain astrocytes</t>
+          <t>placenta hofbauer cells</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>3.195402298850575</v>
+        <v>2.577499867521594</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>adipose tissue schwann cells</t>
+          <t>fallopian tube fibroblasts</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>3.16411842686699</v>
+        <v>2.375</v>
       </c>
     </row>
     <row r="34">
@@ -772,413 +772,413 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>3.137870855148342</v>
+        <v>2.317629179331307</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>fallopian tube neutrophils</t>
+          <t>eye bipolar cells</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>3.112192860454335</v>
+        <v>1.963903743315508</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>immune macrophages</t>
+          <t>liver kupffer cells</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>2.970189098998887</v>
+        <v>1.891176470588235</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>bronchus club cells</t>
+          <t>endometrium glandular and luminal cells</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>2.930359085963003</v>
+        <v>1.797202797202797</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>placenta syncytiotrophoblasts</t>
+          <t>brain microglial cells</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>2.881351200446677</v>
+        <v>1.674761758376883</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>colon undifferentiated cells</t>
+          <t>stomach gastric mucus-secreting cells</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2.772928526249209</v>
+        <v>1.591695501730104</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>testis early spermatids</t>
+          <t>placenta extravillous trophoblasts</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>2.764182424916574</v>
+        <v>1.57843137254902</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>breast breast glandular cells</t>
+          <t>skin langerhans cells</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2.622448979591837</v>
+        <v>1.558469308469308</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>placenta hofbauer cells</t>
+          <t>breast adipocytes</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>2.577499867521594</v>
+        <v>1.475555555555556</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>brain excitatory neurons</t>
+          <t>endometrium endometrial stromal cells</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>2.430675909878683</v>
+        <v>1.428353658536585</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>fallopian tube fibroblasts</t>
+          <t>heart muscle endothelial cells</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>2.375</v>
+        <v>1.405405405405405</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>endometrium glandular and luminal cells</t>
+          <t>salivary gland serous glandular cells</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>2.296855024290462</v>
+        <v>1.279667422524565</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>liver fibroblasts</t>
+          <t>salivary gland mucus glandular cells</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>2.181313296308396</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>testis leydig cells</t>
+          <t>kidney distal tubular cells</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>2.155021834061136</v>
+        <v>1.198012232415902</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>tongue suprabasal keratinocytes</t>
+          <t>liver fibroblasts</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2.05359939378631</v>
+        <v>1.189189189189189</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>eye rod photoreceptor cells</t>
+          <t>adipose tissue adipocytes</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>2.003694848945881</v>
+        <v>1.172686230248307</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>eye bipolar cells</t>
+          <t>immune dendritic cells</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>1.963903743315508</v>
+        <v>1.147727272727273</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>liver kupffer cells</t>
+          <t>skeletal muscle skeletal myocytes</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>1.891176470588235</v>
+        <v>1.022222222222222</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>lung endothelial cells</t>
+          <t>ovary lymphatic endothelial cells</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>1.876211782252051</v>
+        <v>1.018518518518518</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>pancreas ductal cells</t>
+          <t>esophagus smooth muscle cells</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>1.789444749862562</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>immune monocytes</t>
+          <t>heart muscle smooth muscle cells</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>1.678811316914309</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>brain microglial cells</t>
+          <t>bronchus club cells</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>1.674761758376883</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>placenta extravillous trophoblasts</t>
+          <t>bronchus ciliated cells</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>1.630571145592605</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>stomach gastric mucus-secreting cells</t>
+          <t>bronchus basal respiratory cells</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>1.591695501730104</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>small intestine enteroendocrine cells</t>
+          <t>immune monocytes</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>1.572831423895254</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>skeletal muscle skeletal myocytes</t>
+          <t>breast smooth muscle cells</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>1.488789237668162</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>breast adipocytes</t>
+          <t>immune nk-cells</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>1.475555555555556</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>bronchus basal respiratory cells</t>
+          <t>breast fibroblasts</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>1.450598139122729</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>fallopian tube secretory cells</t>
+          <t>breast endothelial cells</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>1.439535803771594</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>endometrium endometrial stromal cells</t>
+          <t>breast breast myoepithelial cells</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>1.428353658536585</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>heart muscle endothelial cells</t>
+          <t>kidney collecting duct cells</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>1.405405405405405</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>adipose tissue smooth muscle cells</t>
+          <t>brain excitatory neurons</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>1.357723577235773</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>salivary gland serous glandular cells</t>
+          <t>bone marrow erythroid cells</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>1.279667422524565</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>salivary gland mucus glandular cells</t>
+          <t>adipose tissue smooth muscle cells</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>kidney distal tubular cells</t>
+          <t>adipose tissue fibroblasts</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>1.198012232415902</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>adipose tissue adipocytes</t>
+          <t>bronchus ionocytes</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>1.172686230248307</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>placenta cytotrophoblasts</t>
+          <t>heart muscle fibroblasts</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>1.129302325581395</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>immune nk-cells</t>
+          <t>esophagus squamous epithelial cells</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>1.055</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>skin langerhans cells</t>
+          <t>fallopian tube endothelial cells</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>1.027289218392618</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>ovary lymphatic endothelial cells</t>
+          <t>esophagus fibroblasts</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>1.018518518518518</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>skin fibroblasts</t>
+          <t>esophagus endothelial cells</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>1.005172413793103</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>endometrium endothelial cells</t>
+          <t>eye horizontal cells</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1188,7 +1188,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>colon enteroendocrine cells</t>
+          <t>liver cholangiocytes</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1198,7 +1198,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>colon intestinal goblet cells</t>
+          <t>eye rod photoreceptor cells</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1208,7 +1208,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>colon paneth cells</t>
+          <t>fallopian tube ciliated cells</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1218,7 +1218,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>testis peritubular cells</t>
+          <t>endometrium smooth muscle cells</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1228,7 +1228,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>endometrium ciliated cells</t>
+          <t>endometrium endothelial cells</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1238,7 +1238,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>rectum distal enterocytes</t>
+          <t>bronchus smooth muscle cells</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1248,7 +1248,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>pancreas endothelial cells</t>
+          <t>endometrium ciliated cells</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1258,7 +1258,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>testis endothelial cells</t>
+          <t>fallopian tube lymphatic endothelial cells</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -1268,7 +1268,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>bronchus smooth muscle cells</t>
+          <t>colon paneth cells</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -1278,7 +1278,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>endometrium smooth muscle cells</t>
+          <t>colon intestinal goblet cells</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -1288,7 +1288,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>esophagus basal squamous epithelial cells</t>
+          <t>fallopian tube secretory cells</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -1298,7 +1298,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>esophagus endothelial cells</t>
+          <t>fallopian tube smooth muscle cells</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -1308,7 +1308,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>esophagus fibroblasts</t>
+          <t>colon enteroendocrine cells</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -1318,7 +1318,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>rectum enteroendocrine cells</t>
+          <t>esophagus basal squamous epithelial cells</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -1328,7 +1328,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>esophagus smooth muscle cells</t>
+          <t>vascular smooth muscle cells</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -1338,7 +1338,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>esophagus squamous epithelial cells</t>
+          <t>liver endothelial cells</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -1348,7 +1348,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>testis sertoli cells</t>
+          <t>salivary gland fibroblasts</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -1358,7 +1358,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>bronchus ionocytes</t>
+          <t>salivary gland smooth muscle cells</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -1368,7 +1368,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>small intestine undifferentiated cells</t>
+          <t>skeletal muscle endothelial cells</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -1378,7 +1378,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>tongue endothelial cells</t>
+          <t>skeletal muscle fibroblasts</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -1388,7 +1388,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>adipose tissue fibroblasts</t>
+          <t>skeletal muscle smooth muscle cells</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -1398,7 +1398,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>vascular fibroblasts</t>
+          <t>skin basal keratinocytes</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -1408,7 +1408,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>prostate endothelial cells</t>
+          <t>skin endothelial cells</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -1418,7 +1418,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>bone marrow erythroid cells</t>
+          <t>skin fibroblasts</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -1428,7 +1428,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>vascular endothelial cells</t>
+          <t>skin smooth muscle cells</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -1438,7 +1438,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>tongue smooth muscle cells</t>
+          <t>small intestine enteroendocrine cells</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -1448,7 +1448,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>tongue serous glandular cells</t>
+          <t>small intestine intestinal goblet cells</t>
         </is>
       </c>
       <c r="B102" t="n">
@@ -1458,7 +1458,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>prostate club cells</t>
+          <t>small intestine paneth cells</t>
         </is>
       </c>
       <c r="B103" t="n">
@@ -1468,7 +1468,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>thymus smooth muscle cells</t>
+          <t>small intestine undifferentiated cells</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -1478,7 +1478,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>testis spermatogonia</t>
+          <t>stomach fibroblasts</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -1488,7 +1488,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>prostate basal prostatic cells</t>
+          <t>testis early spermatids</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -1498,7 +1498,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>thymus mesothelial cells</t>
+          <t>testis endothelial cells</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -1508,7 +1508,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>breast breast myoepithelial cells</t>
+          <t>testis leydig cells</t>
         </is>
       </c>
       <c r="B108" t="n">
@@ -1518,7 +1518,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>breast endothelial cells</t>
+          <t>testis peritubular cells</t>
         </is>
       </c>
       <c r="B109" t="n">
@@ -1528,7 +1528,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>thymus fibroblasts</t>
+          <t>testis sertoli cells</t>
         </is>
       </c>
       <c r="B110" t="n">
@@ -1538,7 +1538,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>breast smooth muscle cells</t>
+          <t>testis spermatogonia</t>
         </is>
       </c>
       <c r="B111" t="n">
@@ -1548,7 +1548,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>prostate smooth muscle cells</t>
+          <t>thymus endothelial cells</t>
         </is>
       </c>
       <c r="B112" t="n">
@@ -1558,7 +1558,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>thymus endothelial cells</t>
+          <t>thymus fibroblasts</t>
         </is>
       </c>
       <c r="B113" t="n">
@@ -1568,7 +1568,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>stomach fibroblasts</t>
+          <t>thymus mesothelial cells</t>
         </is>
       </c>
       <c r="B114" t="n">
@@ -1578,7 +1578,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>small intestine intestinal goblet cells</t>
+          <t>thymus smooth muscle cells</t>
         </is>
       </c>
       <c r="B115" t="n">
@@ -1588,7 +1588,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>eye horizontal cells</t>
+          <t>tongue endothelial cells</t>
         </is>
       </c>
       <c r="B116" t="n">
@@ -1598,7 +1598,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>small intestine paneth cells</t>
+          <t>tongue serous glandular cells</t>
         </is>
       </c>
       <c r="B117" t="n">
@@ -1608,7 +1608,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>liver endothelial cells</t>
+          <t>tongue smooth muscle cells</t>
         </is>
       </c>
       <c r="B118" t="n">
@@ -1618,7 +1618,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>liver erythroid cells</t>
+          <t>tongue suprabasal keratinocytes</t>
         </is>
       </c>
       <c r="B119" t="n">
@@ -1628,7 +1628,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>pancreas fibroblasts</t>
+          <t>vascular endothelial cells</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -1638,7 +1638,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>salivary gland salivary duct cells</t>
+          <t>vascular fibroblasts</t>
         </is>
       </c>
       <c r="B121" t="n">
@@ -1648,7 +1648,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>pancreas exocrine glandular cells</t>
+          <t>salivary gland salivary duct cells</t>
         </is>
       </c>
       <c r="B122" t="n">
@@ -1658,7 +1658,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>liver smooth muscle cells</t>
+          <t>salivary gland endothelial cells</t>
         </is>
       </c>
       <c r="B123" t="n">
@@ -1668,7 +1668,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>salivary gland fibroblasts</t>
+          <t>liver erythroid cells</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -1678,7 +1678,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>salivary gland endothelial cells</t>
+          <t>rectum undifferentiated cells</t>
         </is>
       </c>
       <c r="B125" t="n">
@@ -1688,7 +1688,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>lung ciliated cells</t>
+          <t>liver smooth muscle cells</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -1698,7 +1698,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>lung club cells</t>
+          <t>lung alveolar cells type 1</t>
         </is>
       </c>
       <c r="B127" t="n">
@@ -1708,7 +1708,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>rectum undifferentiated cells</t>
+          <t>lung ciliated cells</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -1718,7 +1718,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>lung fibroblasts</t>
+          <t>lung club cells</t>
         </is>
       </c>
       <c r="B129" t="n">
@@ -1728,7 +1728,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>lung smooth muscle cells</t>
+          <t>lung fibroblasts</t>
         </is>
       </c>
       <c r="B130" t="n">
@@ -1738,7 +1738,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>ovary endothelial cells</t>
+          <t>lung smooth muscle cells</t>
         </is>
       </c>
       <c r="B131" t="n">
@@ -1748,7 +1748,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>ovary granulosa cells</t>
+          <t>ovary endothelial cells</t>
         </is>
       </c>
       <c r="B132" t="n">
@@ -1758,7 +1758,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>rectum paneth cells</t>
+          <t>ovary granulosa cells</t>
         </is>
       </c>
       <c r="B133" t="n">
@@ -1778,7 +1778,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>liver cholangiocytes</t>
+          <t>ovary smooth muscle cells</t>
         </is>
       </c>
       <c r="B135" t="n">
@@ -1788,7 +1788,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>salivary gland smooth muscle cells</t>
+          <t>pancreas ductal cells</t>
         </is>
       </c>
       <c r="B136" t="n">
@@ -1798,7 +1798,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>pancreas pancreatic endocrine cells</t>
+          <t>pancreas endothelial cells</t>
         </is>
       </c>
       <c r="B137" t="n">
@@ -1808,7 +1808,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>prostate fibroblasts</t>
+          <t>pancreas exocrine glandular cells</t>
         </is>
       </c>
       <c r="B138" t="n">
@@ -1818,7 +1818,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>ovary smooth muscle cells</t>
+          <t>pancreas fibroblasts</t>
         </is>
       </c>
       <c r="B139" t="n">
@@ -1828,7 +1828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>fallopian tube ciliated cells</t>
+          <t>pancreas pancreatic endocrine cells</t>
         </is>
       </c>
       <c r="B140" t="n">
@@ -1838,7 +1838,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>fallopian tube endothelial cells</t>
+          <t>placenta cytotrophoblasts</t>
         </is>
       </c>
       <c r="B141" t="n">
@@ -1848,7 +1848,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>placenta fibroblasts</t>
+          <t>placenta endothelial cells</t>
         </is>
       </c>
       <c r="B142" t="n">
@@ -1858,7 +1858,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>fallopian tube lymphatic endothelial cells</t>
+          <t>placenta fibroblasts</t>
         </is>
       </c>
       <c r="B143" t="n">
@@ -1868,7 +1868,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>placenta endothelial cells</t>
+          <t>placenta smooth muscle cells</t>
         </is>
       </c>
       <c r="B144" t="n">
@@ -1878,7 +1878,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>fallopian tube smooth muscle cells</t>
+          <t>prostate basal prostatic cells</t>
         </is>
       </c>
       <c r="B145" t="n">
@@ -1888,7 +1888,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>heart muscle fibroblasts</t>
+          <t>prostate club cells</t>
         </is>
       </c>
       <c r="B146" t="n">
@@ -1898,7 +1898,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>kidney collecting duct cells</t>
+          <t>prostate endothelial cells</t>
         </is>
       </c>
       <c r="B147" t="n">
@@ -1908,7 +1908,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>heart muscle smooth muscle cells</t>
+          <t>prostate fibroblasts</t>
         </is>
       </c>
       <c r="B148" t="n">
@@ -1918,7 +1918,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>skin endothelial cells</t>
+          <t>prostate prostatic glandular cells</t>
         </is>
       </c>
       <c r="B149" t="n">
@@ -1928,7 +1928,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>skin basal keratinocytes</t>
+          <t>prostate smooth muscle cells</t>
         </is>
       </c>
       <c r="B150" t="n">
@@ -1938,7 +1938,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>skeletal muscle smooth muscle cells</t>
+          <t>rectum distal enterocytes</t>
         </is>
       </c>
       <c r="B151" t="n">
@@ -1948,7 +1948,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>rectum intestinal goblet cells</t>
+          <t>rectum enteroendocrine cells</t>
         </is>
       </c>
       <c r="B152" t="n">
@@ -1958,7 +1958,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>skeletal muscle fibroblasts</t>
+          <t>rectum intestinal goblet cells</t>
         </is>
       </c>
       <c r="B153" t="n">
@@ -1968,7 +1968,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>skeletal muscle endothelial cells</t>
+          <t>rectum paneth cells</t>
         </is>
       </c>
       <c r="B154" t="n">
@@ -1978,7 +1978,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>prostate prostatic glandular cells</t>
+          <t>lung endothelial cells</t>
         </is>
       </c>
       <c r="B155" t="n">

</xml_diff>